<commit_message>
Added test case fix 23 February 2018 at 13:31:39 CET - Vignesh Renganathan / When reading the empty cell. the app crashes
</commit_message>
<xml_diff>
--- a/XlsxReaderWriterTests/testWorkbook.xlsx
+++ b/XlsxReaderWriterTests/testWorkbook.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/renebigot/Documents/iPhone/Drafts/Sondage/XlsxReaderWriter/XlsxReaderWriterTests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dm/git/XlsxReaderWriter/XlsxReaderWriterTests/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE9F988-6E5D-3147-925D-534C5677BCCC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
+    <workbookView xWindow="-24720" yWindow="3400" windowWidth="22400" windowHeight="12660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Utilisateur de Microsoft Office</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0">
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Number</t>
   </si>
@@ -122,11 +123,14 @@
   <si>
     <t>Grouped cell</t>
   </si>
+  <si>
+    <t>Formatted Cell</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[mm]:ss"/>
     <numFmt numFmtId="165" formatCode="[ss]"/>
@@ -180,7 +184,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14996795556505021"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -222,7 +232,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -233,18 +243,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -252,6 +263,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -274,7 +288,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -312,7 +332,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -658,11 +684,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28:F39"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +791,7 @@
       </c>
       <c r="B7" s="1">
         <f ca="1">TODAY()</f>
-        <v>42331</v>
+        <v>43155</v>
       </c>
       <c r="D7">
         <v>7</v>
@@ -803,6 +829,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="8"/>
       <c r="D12">
         <v>12</v>
       </c>

</xml_diff>